<commit_message>
Used new MD predictions excel.
</commit_message>
<xml_diff>
--- a/breakfast/670G Fiasp Subject Dates.xlsx
+++ b/breakfast/670G Fiasp Subject Dates.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share$/Endo/Buckingham Studies/1. Active studies/46202 - Fiasp 670G/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinwang/Documents/Stanford/Research/breakfast/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF801434-8A04-7342-89F2-384E26476488}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="4140" windowWidth="24960" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="24960" windowHeight="13960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Subject ID</t>
   </si>
   <si>
-    <t>Insulin 1</t>
-  </si>
-  <si>
     <t>Meal Dates</t>
   </si>
   <si>
@@ -44,9 +42,6 @@
     <t>Week 2</t>
   </si>
   <si>
-    <t>Insulin 2</t>
-  </si>
-  <si>
     <t>670GF101</t>
   </si>
   <si>
@@ -92,9 +87,6 @@
     <t>08/29-08/31</t>
   </si>
   <si>
-    <t>09/11-09-13</t>
-  </si>
-  <si>
     <t>09/24-09/26</t>
   </si>
   <si>
@@ -123,12 +115,24 @@
   </si>
   <si>
     <t>10/21-10/23</t>
+  </si>
+  <si>
+    <t>insulin 1 is first use of a blinded insulin</t>
+  </si>
+  <si>
+    <t>insulin 2 is second use of a blinded insulin</t>
+  </si>
+  <si>
+    <t>2nd insulin</t>
+  </si>
+  <si>
+    <t>1st insulin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -158,16 +162,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,6 +184,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -444,313 +454,319 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" s="2">
+        <v>43329</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43336</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43343</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43350</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43329</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43336</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>43343</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43350</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B5" s="2">
         <v>43329</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C5" s="2">
         <v>43336</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>43343</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43350</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43341</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43349</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2">
+        <v>43356</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43363</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43349</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43356</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3">
-        <v>43343</v>
-      </c>
-      <c r="F3" s="3">
-        <v>43350</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>43329</v>
-      </c>
-      <c r="C4" s="3">
-        <v>43336</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3">
-        <v>43343</v>
-      </c>
-      <c r="F4" s="3">
-        <v>43350</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>43329</v>
-      </c>
-      <c r="C5" s="3">
-        <v>43336</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3">
-        <v>43343</v>
-      </c>
-      <c r="F5" s="3">
-        <v>43350</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E7" s="2">
+        <v>43363</v>
+      </c>
+      <c r="F7" s="2">
+        <v>43370</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
-        <v>43341</v>
-      </c>
-      <c r="C6" s="3">
-        <v>43349</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B8" s="2">
+        <v>43365</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43372</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2">
+        <v>43379</v>
+      </c>
+      <c r="F8" s="2">
+        <v>43386</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
         <v>43356</v>
       </c>
-      <c r="F6" s="3">
+      <c r="C9" s="2">
         <v>43363</v>
       </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3">
-        <v>43349</v>
-      </c>
-      <c r="C7" s="3">
-        <v>43356</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3">
-        <v>43363</v>
-      </c>
-      <c r="F7" s="3">
-        <v>43370</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="E9" s="2">
+        <v>43371</v>
+      </c>
+      <c r="F9" s="2">
+        <v>43378</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
-        <v>43365</v>
-      </c>
-      <c r="C8" s="3">
-        <v>43372</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="3">
-        <v>43379</v>
-      </c>
-      <c r="F8" s="3">
-        <v>43386</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B10" s="2">
+        <v>43371</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43378</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="E10" s="2">
+        <v>43385</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43392</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3">
-        <v>43356</v>
-      </c>
-      <c r="C9" s="3">
-        <v>43363</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="3">
-        <v>43371</v>
-      </c>
-      <c r="F9" s="3">
-        <v>43378</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="B11" s="2">
+        <v>43369</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43376</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2">
+        <v>43384</v>
+      </c>
+      <c r="F11" s="2">
+        <v>43391</v>
+      </c>
+      <c r="G11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3">
-        <v>43371</v>
-      </c>
-      <c r="C10" s="3">
-        <v>43378</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="3">
-        <v>43385</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="B12" s="2">
+        <v>43368</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43375</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>43382</v>
+      </c>
+      <c r="F12" s="2">
+        <v>43389</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43377</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43384</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
         <v>43392</v>
       </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3">
-        <v>43369</v>
-      </c>
-      <c r="C11" s="3">
-        <v>43376</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="3">
-        <v>43384</v>
-      </c>
-      <c r="F11" s="3">
-        <v>43391</v>
-      </c>
-      <c r="G11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="F13" s="2">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3">
-        <v>43368</v>
-      </c>
-      <c r="C12" s="3">
-        <v>43375</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3">
-        <v>43382</v>
-      </c>
-      <c r="F12" s="3">
-        <v>43389</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3">
-        <v>43377</v>
-      </c>
-      <c r="C13" s="3">
-        <v>43384</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3">
-        <v>43392</v>
-      </c>
-      <c r="F13" s="3">
-        <v>43399</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>43388</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>43395</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
         <v>43402</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>